<commit_message>
importar 2 salto a la vista
</commit_message>
<xml_diff>
--- a/public/files/example/importar_facturas_clientes_emizor.xlsx
+++ b/public/files/example/importar_facturas_clientes_emizor.xlsx
@@ -389,9 +389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>